<commit_message>
Allow date converter to specify several columns.
</commit_message>
<xml_diff>
--- a/DECS Excel Add-Ins/test files/dummy_data_for_formatting.xlsx
+++ b/DECS Excel Add-Ins/test files/dummy_data_for_formatting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\DECS-Office-AddIns\DECS Excel Add-Ins\test files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C536AC5-1538-4DE6-8B57-34EAFE0D1DEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13B3F45-9654-4316-947F-FC5E081A806D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{9009A106-12E3-43A0-920B-9305A21EC74D}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Gertrude George</t>
+  </si>
+  <si>
+    <t>Bob</t>
   </si>
 </sst>
 </file>
@@ -538,13 +541,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E27030-8E9B-4660-B21D-AB08C362F56E}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -570,6 +576,16 @@
         <v>32301</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>27945</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>